<commit_message>
Added CIFAR100 results for ResNet-18
</commit_message>
<xml_diff>
--- a/MTD_2025.xlsx
+++ b/MTD_2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\Vscode\Projects\MTD_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E0B734-2478-48D4-8FBB-8BB81833264B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736180F3-F6F4-4CEA-92B7-FEADE24E72CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,31 +19,10 @@
     <sheet name="CIFAR100" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">(CIFAR10!$A$7:$A$11,CIFAR10!$A$14:$A$18,CIFAR10!$A$21:$A$25)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">(CIFAR10!$F$7:$F$11,CIFAR10!$F$14:$F$18,CIFAR10!$F$21:$F$25)</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">GLOBAL!$N$6:$N$20</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">GLOBAL!$O$6:$O$20</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">(CIFAR10!$A$7,CIFAR10!$A$14)</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">(CIFAR10!$A$7,CIFAR10!$A$14,CIFAR10!$A$21)</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">(CIFAR10!$A$7:$A$11,CIFAR10!$A$14:$A$18)</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">(CIFAR10!$A$7:$A$11,CIFAR10!$A$14:$A$18,CIFAR10!$A$21:$A$25)</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">(CIFAR10!$F$7:$F$11,CIFAR10!$F$14:$F$17)</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">(CIFAR10!$F$7:$F$11,CIFAR10!$F$14:$F$18)</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">(CIFAR10!$F$7:$F$11,CIFAR10!$F$14:$F$18,CIFAR10!$F$21:$F$25)</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">CIFAR10!$A$7</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">(CIFAR100!$F$7:$F$11,CIFAR100!$F$14:$F$18,CIFAR100!$F$21:$F$25)</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">CIFAR10!$A$7:$A$27</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">CIFAR10!$F$14:$F$18</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">CIFAR10!$F$6</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">CIFAR10!$F$7:$F$11</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">CIFAR10!$F$7:$F$27</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">CIFAR10!$F$6</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">GLOBAL!$L$6:$L$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">GLOBAL!$M$6:$M$20</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">GLOBAL!$N$6:$N$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">GLOBAL!$O$6:$O$20</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">GLOBAL!$L$6:$L$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">GLOBAL!$M$6:$M$20</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">GLOBAL!$L$6:$L$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">GLOBAL!$M$6:$M$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">GLOBAL!$N$6:$N$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">GLOBAL!$O$6:$O$20</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -256,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -413,6 +392,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -423,7 +457,7 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -438,9 +472,7 @@
     <xf numFmtId="10" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
@@ -454,27 +486,33 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="5"/>
     <xf numFmtId="10" fontId="9" fillId="9" borderId="7" xfId="5" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="16" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="15" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -541,6 +579,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <font>
@@ -559,7 +598,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -579,26 +617,26 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.10</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -636,6 +674,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{1AB7D9E8-D4E2-4C72-BDC5-A9AD95EE95B0}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>MLP</cx:v>
             </cx:txData>
           </cx:tx>
@@ -648,6 +687,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{AAAD8E81-5775-481F-B473-FCE4DA44872C}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>CNN</cx:v>
             </cx:txData>
           </cx:tx>
@@ -660,6 +700,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{A1F3E258-8243-4130-94C8-F09ED292F634}">
           <cx:tx>
             <cx:txData>
+              <cx:f/>
               <cx:v>RESNET</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1271,8 +1312,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1499938" y="689810"/>
-              <a:ext cx="4572000" cy="2743200"/>
+              <a:off x="1499938" y="684997"/>
+              <a:ext cx="4572000" cy="2719137"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1306,13 +1347,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E212CE2C-A200-49AB-9B6B-A1462F2A19E9}" name="Table2" displayName="Table2" ref="L5:O20" totalsRowShown="0" dataDxfId="2" dataCellStyle="Percent">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E212CE2C-A200-49AB-9B6B-A1462F2A19E9}" name="Table2" displayName="Table2" ref="L5:O20" totalsRowShown="0" dataDxfId="3" dataCellStyle="Percent">
   <autoFilter ref="L5:O20" xr:uid="{E212CE2C-A200-49AB-9B6B-A1462F2A19E9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{DF8591C0-BA9E-48F6-873B-CBE8216B9F8E}" name="NN"/>
-    <tableColumn id="2" xr3:uid="{17A7B3B9-E69D-4263-89AD-CE3FCF97694A}" name="MLP" dataDxfId="1" dataCellStyle="Percent"/>
-    <tableColumn id="3" xr3:uid="{645DD193-BFB7-4046-AB3A-FE0027D101AB}" name="CNN" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="4" xr3:uid="{E3F2AD4B-483D-4819-8B6E-21E26C9EDC0F}" name="RESNET" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="2" xr3:uid="{17A7B3B9-E69D-4263-89AD-CE3FCF97694A}" name="MLP" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="3" xr3:uid="{645DD193-BFB7-4046-AB3A-FE0027D101AB}" name="CNN" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="4" xr3:uid="{E3F2AD4B-483D-4819-8B6E-21E26C9EDC0F}" name="RESNET" dataDxfId="0" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1638,7 +1679,7 @@
   <dimension ref="L5:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C2" zoomScale="92" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29:O41"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,7 +1709,7 @@
       <c r="M6" s="2">
         <v>0.95796999999999999</v>
       </c>
-      <c r="N6" s="44">
+      <c r="N6" s="35">
         <v>0.97799999999999998</v>
       </c>
     </row>
@@ -1679,7 +1720,7 @@
       <c r="M7" s="2">
         <v>0.95104999999999995</v>
       </c>
-      <c r="N7" s="44">
+      <c r="N7" s="35">
         <v>0.96951670000000001</v>
       </c>
     </row>
@@ -1690,7 +1731,7 @@
       <c r="M8" s="2">
         <v>0.94906000000000001</v>
       </c>
-      <c r="N8" s="44">
+      <c r="N8" s="35">
         <v>0.98361670000000001</v>
       </c>
     </row>
@@ -1701,7 +1742,7 @@
       <c r="M9" s="2">
         <v>0.95250000000000001</v>
       </c>
-      <c r="N9" s="44">
+      <c r="N9" s="35">
         <v>0.98463400000000001</v>
       </c>
     </row>
@@ -1712,7 +1753,7 @@
       <c r="M10" s="2">
         <v>0.96092</v>
       </c>
-      <c r="N10" s="44">
+      <c r="N10" s="35">
         <v>0.98465000000000003</v>
       </c>
     </row>
@@ -1720,10 +1761,10 @@
       <c r="L11" t="s">
         <v>15</v>
       </c>
-      <c r="M11" s="44">
+      <c r="M11" s="35">
         <v>0.42558000000000001</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="35">
         <v>0.59211999999999998</v>
       </c>
     </row>
@@ -1731,10 +1772,10 @@
       <c r="L12" t="s">
         <v>15</v>
       </c>
-      <c r="M12" s="44">
+      <c r="M12" s="35">
         <v>0.4219</v>
       </c>
-      <c r="N12" s="44">
+      <c r="N12" s="35">
         <v>0.59199999999999997</v>
       </c>
     </row>
@@ -1742,10 +1783,10 @@
       <c r="L13" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="44">
+      <c r="M13" s="35">
         <v>0.42796000000000001</v>
       </c>
-      <c r="N13" s="44">
+      <c r="N13" s="35">
         <v>0.59275999999999995</v>
       </c>
     </row>
@@ -1753,10 +1794,10 @@
       <c r="L14" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="44">
+      <c r="M14" s="35">
         <v>0.43668000000000001</v>
       </c>
-      <c r="N14" s="44">
+      <c r="N14" s="35">
         <v>0.59489999999999998</v>
       </c>
     </row>
@@ -1764,10 +1805,10 @@
       <c r="L15" t="s">
         <v>15</v>
       </c>
-      <c r="M15" s="44">
+      <c r="M15" s="35">
         <v>0.42558000000000001</v>
       </c>
-      <c r="N15" s="44">
+      <c r="N15" s="35">
         <v>0.57767999999999997</v>
       </c>
     </row>
@@ -1775,63 +1816,71 @@
       <c r="L16" t="s">
         <v>16</v>
       </c>
-      <c r="M16" s="44">
+      <c r="M16" s="35">
         <v>0.14152000000000001</v>
       </c>
-      <c r="N16" s="44">
+      <c r="N16" s="35">
         <v>0.21504000000000001</v>
       </c>
-      <c r="O16" s="44">
-        <v>0.34477999999999998</v>
+      <c r="O16" s="35">
+        <v>0.31286000000000003</v>
       </c>
     </row>
     <row r="17" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L17" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="44">
+      <c r="M17" s="35">
         <v>0.14566000000000001</v>
       </c>
-      <c r="N17" s="44">
+      <c r="N17" s="35">
         <v>0.20785999999999999</v>
       </c>
-      <c r="O17" s="44"/>
+      <c r="O17" s="35">
+        <v>0.32181999999999999</v>
+      </c>
     </row>
     <row r="18" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L18" t="s">
         <v>16</v>
       </c>
-      <c r="M18" s="44">
+      <c r="M18" s="35">
         <v>0.1484</v>
       </c>
-      <c r="N18" s="44">
+      <c r="N18" s="35">
         <v>0.20391999999999999</v>
       </c>
-      <c r="O18" s="44"/>
+      <c r="O18" s="35">
+        <v>0.3165</v>
+      </c>
     </row>
     <row r="19" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L19" t="s">
         <v>16</v>
       </c>
-      <c r="M19" s="44">
+      <c r="M19" s="35">
         <v>0.15104000000000001</v>
       </c>
-      <c r="N19" s="44">
+      <c r="N19" s="35">
         <v>0.2059</v>
       </c>
-      <c r="O19" s="44"/>
+      <c r="O19" s="35">
+        <v>0.33235999999999999</v>
+      </c>
     </row>
     <row r="20" spans="12:15" x14ac:dyDescent="0.3">
       <c r="L20" t="s">
         <v>16</v>
       </c>
-      <c r="M20" s="44">
+      <c r="M20" s="35">
         <v>0.15068000000000001</v>
       </c>
-      <c r="N20" s="44">
+      <c r="N20" s="35">
         <v>0.20172000000000001</v>
       </c>
-      <c r="O20" s="44"/>
+      <c r="O20" s="35">
+        <v>0.31991999999999998</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -1847,8 +1896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F18"/>
+    <sheetView zoomScale="71" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,36 +1914,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="29">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="48" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>1</v>
       </c>
       <c r="C7">
@@ -1907,15 +1956,15 @@
         <f>C7*D7</f>
         <v>645.86260000000004</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="37">
         <v>0.97799999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="21">
         <v>2</v>
       </c>
       <c r="C8">
@@ -1928,15 +1977,15 @@
         <f t="shared" ref="E8:E11" si="0">C8*D8</f>
         <v>646.6404</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="37">
         <v>0.96951670000000001</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="21">
         <v>3</v>
       </c>
       <c r="C9">
@@ -1949,15 +1998,15 @@
         <f t="shared" si="0"/>
         <v>652.29919999999993</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="37">
         <v>0.98361670000000001</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10" s="21">
         <v>4</v>
       </c>
       <c r="C10">
@@ -1970,15 +2019,15 @@
         <f t="shared" si="0"/>
         <v>686.78399999999999</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="37">
         <v>0.98463400000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="23">
+      <c r="B11" s="21">
         <v>5</v>
       </c>
       <c r="C11">
@@ -1991,13 +2040,12 @@
         <f t="shared" si="0"/>
         <v>662.71040000000005</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="37">
         <v>0.98465000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="6">
@@ -2012,14 +2060,13 @@
         <f t="shared" si="1"/>
         <v>658.85932000000003</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="39">
         <f t="shared" si="1"/>
         <v>0.98008348000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="8">
@@ -2034,16 +2081,16 @@
         <f t="shared" si="2"/>
         <v>16.999047630735081</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="40">
         <f t="shared" si="2"/>
         <v>6.5200020940947611E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="21">
         <v>1</v>
       </c>
       <c r="C14" s="10">
@@ -2056,15 +2103,15 @@
         <f>C14*D14</f>
         <v>472.3494</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="43">
         <v>0.95796999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="21">
         <v>2</v>
       </c>
       <c r="C15" s="10">
@@ -2077,15 +2124,15 @@
         <f t="shared" ref="E15:E18" si="3">C15*D15</f>
         <v>490.38990000000001</v>
       </c>
-      <c r="F15" s="39">
+      <c r="F15" s="43">
         <v>0.95104999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="21">
         <v>3</v>
       </c>
       <c r="C16" s="10">
@@ -2098,15 +2145,15 @@
         <f t="shared" si="3"/>
         <v>496.52519999999998</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="43">
         <v>0.94906000000000001</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="23">
+      <c r="B17" s="21">
         <v>4</v>
       </c>
       <c r="C17" s="10">
@@ -2119,15 +2166,15 @@
         <f t="shared" si="3"/>
         <v>488.34199999999998</v>
       </c>
-      <c r="F17" s="39">
+      <c r="F17" s="43">
         <v>0.95250000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="21">
         <v>5</v>
       </c>
       <c r="C18" s="10">
@@ -2140,13 +2187,12 @@
         <f t="shared" si="3"/>
         <v>506.02140000000003</v>
       </c>
-      <c r="F18" s="39">
+      <c r="F18" s="43">
         <v>0.96092</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="11">
@@ -2161,96 +2207,94 @@
         <f t="shared" si="4"/>
         <v>490.72557999999998</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="44">
         <f t="shared" si="4"/>
         <v>0.95430000000000015</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="12">
         <f>_xlfn.STDEV.S(C14:C18)</f>
         <v>0.77811072476865384</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="12">
         <f t="shared" ref="D20:F20" si="5">_xlfn.STDEV.S(D14:D18)</f>
         <v>0.48270073544588643</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <f t="shared" si="5"/>
         <v>12.359973985490429</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="45">
         <f t="shared" si="5"/>
         <v>4.9637032546275359E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B21" s="21">
         <v>1</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="40"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="46"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="21">
         <v>2</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="40"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="46"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="21">
         <v>3</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="40"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="46"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="21">
         <v>4</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="40"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="46"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="21">
         <v>5</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="40"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="46"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="11" t="e">
@@ -2265,29 +2309,28 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F26" s="12" t="e">
+      <c r="F26" s="44" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="13" t="e">
+      <c r="C27" s="12" t="e">
         <f>_xlfn.STDEV.S(C21:C25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D27" s="13" t="e">
+      <c r="D27" s="12" t="e">
         <f t="shared" ref="D27:F27" si="7">_xlfn.STDEV.S(D21:D25)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E27" s="13" t="e">
+      <c r="E27" s="12" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F27" s="14" t="e">
+      <c r="F27" s="45" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
@@ -2305,12 +2348,12 @@
       <c r="A31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="36" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="41"/>
+      <c r="A33" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2325,7 +2368,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F19" sqref="F19:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2339,35 +2382,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="27">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
       <c r="C7" s="3">
@@ -2385,10 +2428,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8">
@@ -2406,10 +2449,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="17">
         <v>3</v>
       </c>
       <c r="C9">
@@ -2427,10 +2470,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="17">
         <v>4</v>
       </c>
       <c r="C10">
@@ -2448,10 +2491,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="17">
         <v>5</v>
       </c>
       <c r="C11">
@@ -2469,8 +2512,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="6">
@@ -2491,8 +2533,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="8">
@@ -2513,10 +2554,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="17">
         <v>1</v>
       </c>
       <c r="C14">
@@ -2534,10 +2575,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="17">
         <v>2</v>
       </c>
       <c r="C15">
@@ -2555,10 +2596,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <v>3</v>
       </c>
       <c r="C16">
@@ -2576,10 +2617,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>4</v>
       </c>
       <c r="C17">
@@ -2597,10 +2638,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="17">
         <v>5</v>
       </c>
       <c r="C18">
@@ -2618,8 +2659,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="6">
@@ -2634,14 +2674,13 @@
         <f t="shared" si="4"/>
         <v>2637.1577599999996</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="39">
         <f t="shared" si="4"/>
         <v>0.42754000000000003</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="8">
@@ -2656,74 +2695,73 @@
         <f t="shared" si="5"/>
         <v>37.44404780079185</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="40">
         <f t="shared" si="5"/>
         <v>5.5499729729071691E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="17">
         <v>1</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="36"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="17">
         <v>2</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="17">
         <v>3</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="17">
         <v>4</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <v>5</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="6" t="e">
@@ -2738,14 +2776,13 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F26" s="6" t="e">
+      <c r="F26" s="41" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="8" t="e">
@@ -2760,18 +2797,18 @@
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F27" s="8" t="e">
+      <c r="F27" s="42" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="36" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="41"/>
+      <c r="A33" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2786,8 +2823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F031AD8A-BB72-41E4-8544-02A77C3204F0}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2801,35 +2838,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="27">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="16">
         <v>1</v>
       </c>
       <c r="C7" s="3">
@@ -2847,10 +2884,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8">
@@ -2868,10 +2905,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="17">
         <v>3</v>
       </c>
       <c r="C9">
@@ -2889,10 +2926,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="17">
         <v>4</v>
       </c>
       <c r="C10">
@@ -2910,10 +2947,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="17">
         <v>5</v>
       </c>
       <c r="C11">
@@ -2931,8 +2968,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="6">
@@ -2953,8 +2989,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="8">
@@ -2975,10 +3010,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="17">
         <v>1</v>
       </c>
       <c r="C14">
@@ -2996,10 +3031,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="17">
         <v>2</v>
       </c>
       <c r="C15">
@@ -3017,10 +3052,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <v>3</v>
       </c>
       <c r="C16">
@@ -3038,10 +3073,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>4</v>
       </c>
       <c r="C17">
@@ -3059,10 +3094,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="17">
         <v>5</v>
       </c>
       <c r="C18">
@@ -3080,8 +3115,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="6">
@@ -3096,14 +3130,13 @@
         <f t="shared" si="4"/>
         <v>6539.4498999999996</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="39">
         <f t="shared" si="4"/>
         <v>0.14745999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="8">
@@ -3118,131 +3151,165 @@
         <f t="shared" si="5"/>
         <v>159.10020015004687</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="40">
         <f t="shared" si="5"/>
         <v>3.9557553008243568E-3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="17">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>5216.34</v>
+        <v>5112.71</v>
       </c>
       <c r="D21">
-        <v>63.8</v>
+        <v>65.3</v>
       </c>
       <c r="E21">
         <f>C21*D21</f>
-        <v>332802.49199999997</v>
+        <v>333859.96299999999</v>
       </c>
       <c r="F21" s="5">
-        <v>0.34477999999999998</v>
+        <v>0.31286000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
+      <c r="A22" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="17">
         <v>2</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
+      <c r="C22">
+        <v>5120.29</v>
+      </c>
+      <c r="D22">
+        <v>63.7</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E25" si="6">C22*D22</f>
+        <v>326162.473</v>
+      </c>
+      <c r="F22" s="37">
+        <v>0.32181999999999999</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="17">
         <v>3</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
+      <c r="C23">
+        <v>5110.3599999999997</v>
+      </c>
+      <c r="D23">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="6"/>
+        <v>340349.97599999997</v>
+      </c>
+      <c r="F23" s="37">
+        <v>0.3165</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="17">
         <v>4</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
+      <c r="C24">
+        <v>5111.1000000000004</v>
+      </c>
+      <c r="D24">
+        <v>62.4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="6"/>
+        <v>318932.64</v>
+      </c>
+      <c r="F24" s="37">
+        <v>0.33235999999999999</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <v>5</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
+      <c r="C25">
+        <v>5107.63</v>
+      </c>
+      <c r="D25">
+        <v>60.7</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="6"/>
+        <v>310033.141</v>
+      </c>
+      <c r="F25" s="38">
+        <v>0.31991999999999998</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="43"/>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="18" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="6">
         <f>AVERAGE(C21:C25)</f>
-        <v>5216.34</v>
+        <v>5112.4179999999997</v>
       </c>
       <c r="D26" s="6">
         <f>AVERAGE(D21:D25)</f>
-        <v>63.8</v>
+        <v>63.739999999999995</v>
       </c>
       <c r="E26" s="6">
-        <f t="shared" ref="E26:F26" si="6">AVERAGE(E21:E25)</f>
-        <v>332802.49199999997</v>
-      </c>
-      <c r="F26" s="33">
-        <f t="shared" si="6"/>
-        <v>0.34477999999999998</v>
+        <f t="shared" ref="E26:F26" si="7">AVERAGE(E21:E25)</f>
+        <v>325867.63860000006</v>
+      </c>
+      <c r="F26" s="39">
+        <f t="shared" si="7"/>
+        <v>0.32069199999999998</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="43"/>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="8" t="e">
+      <c r="C27" s="8">
         <f>_xlfn.STDEV.S(C21:C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D27" s="8" t="e">
+        <v>4.7684137823808559</v>
+      </c>
+      <c r="D27" s="8">
         <f>_xlfn.STDEV.S(D21:D25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E27" s="8" t="e">
-        <f t="shared" ref="E27:F27" si="7">_xlfn.STDEV.S(E21:E25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="34" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>2.3265854809140336</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" ref="E27:F27" si="8">_xlfn.STDEV.S(E21:E25)</f>
+        <v>11963.776504851048</v>
+      </c>
+      <c r="F27" s="40">
+        <f t="shared" si="8"/>
+        <v>7.3641645826257734E-3</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="36" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="41"/>
+      <c r="A33" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>